<commit_message>
Username replaced with Team
</commit_message>
<xml_diff>
--- a/final_teams.xlsx
+++ b/final_teams.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,20 +447,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -469,96 +464,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sf61561(Syed Fahad Mahmud)</t>
+          <t>Tamjid_Hossen(Tamjid)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C2" t="n">
         <v>300</v>
       </c>
       <c r="D2" t="n">
-        <v>300</v>
-      </c>
-      <c r="E2" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>y_this_kolaveri(SAIF)</t>
+          <t>YouDOntKNowWHo(Nabeel Ahsan)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="C3" t="n">
         <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>258</v>
-      </c>
-      <c r="E3" t="n">
-        <v>774</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YouDOntKNowWHo(Nabeel Ahsan)</t>
+          <t>sf61561(Syed Fahad Mahmud)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="C4" t="n">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="D4" t="n">
-        <v>225</v>
-      </c>
-      <c r="E4" t="n">
-        <v>675</v>
+        <v>464</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tamjid_Hossen(Tamjid)</t>
+          <t>shazidmashrafi(Shazid)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C5" t="n">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="D5" t="n">
-        <v>200</v>
-      </c>
-      <c r="E5" t="n">
-        <v>506</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>shazidmashrafi(Shazid)</t>
+          <t>y_this_kolaveri(SAIF)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="C6" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D6" t="n">
-        <v>180</v>
-      </c>
-      <c r="E6" t="n">
-        <v>460</v>
+        <v>378</v>
       </c>
     </row>
     <row r="7">
@@ -574,10 +554,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="n">
-        <v>129</v>
-      </c>
-      <c r="E7" t="n">
-        <v>458</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8">
@@ -590,165 +567,138 @@
         <v>164</v>
       </c>
       <c r="C8" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="D8" t="n">
-        <v>164</v>
-      </c>
-      <c r="E8" t="n">
-        <v>423</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Aniksamiul(Anik)</t>
+          <t>rakin_ahsan(Rakin)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C9" t="n">
         <v>180</v>
       </c>
       <c r="D9" t="n">
-        <v>120</v>
-      </c>
-      <c r="E9" t="n">
-        <v>420</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Marufhussain(maruf)</t>
+          <t>farhanshadiq(Farhan)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="C10" t="n">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="D10" t="n">
-        <v>150</v>
-      </c>
-      <c r="E10" t="n">
-        <v>390</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>farhanshadiq(Farhan)</t>
+          <t>Noornabi1770(Noor)</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C11" t="n">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D11" t="n">
-        <v>113</v>
-      </c>
-      <c r="E11" t="n">
-        <v>390</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Akash_khan</t>
+          <t>Aniksamiul(Anik)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C12" t="n">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D12" t="n">
-        <v>139</v>
-      </c>
-      <c r="E12" t="n">
-        <v>364</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>rakin_ahsan(Rakin)</t>
+          <t>Apon_Chowdhury(Apon)</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C13" t="n">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D13" t="n">
-        <v>106</v>
-      </c>
-      <c r="E13" t="n">
-        <v>362</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Apon_Chowdhury(Apon)</t>
+          <t>Marufhussain(maruf)</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C14" t="n">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>100</v>
-      </c>
-      <c r="E14" t="n">
-        <v>339</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>SadmanIshtiak(Sadman)</t>
+          <t>Akash_khan</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C15" t="n">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>95</v>
-      </c>
-      <c r="E15" t="n">
-        <v>319</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Noornabi1770(Noor)</t>
+          <t>SadmanIshtiak(Sadman)</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C16" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
-      </c>
-      <c r="E16" t="n">
-        <v>300</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17">
@@ -761,13 +711,10 @@
         <v>86</v>
       </c>
       <c r="C17" t="n">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>86</v>
-      </c>
-      <c r="E17" t="n">
-        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +728,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,20 +744,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -819,58 +761,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sf61561(Syed Fahad Mahmud)</t>
+          <t>Tamjid_Hossen(Tamjid)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C2" t="n">
         <v>300</v>
       </c>
       <c r="D2" t="n">
-        <v>300</v>
-      </c>
-      <c r="E2" t="n">
-        <v>900</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>y_this_kolaveri(SAIF)</t>
+          <t>YouDOntKNowWHo(Nabeel Ahsan)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="C3" t="n">
         <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>258</v>
-      </c>
-      <c r="E3" t="n">
-        <v>774</v>
+        <v>483</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>YouDOntKNowWHo(Nabeel Ahsan)</t>
+          <t>sf61561(Syed Fahad Mahmud)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>225</v>
+        <v>300</v>
       </c>
       <c r="C4" t="n">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="D4" t="n">
-        <v>225</v>
-      </c>
-      <c r="E4" t="n">
-        <v>675</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -884,7 +817,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -900,20 +833,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -922,39 +850,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tamjid_Hossen(Tamjid)</t>
+          <t>shazidmashrafi(Shazid)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C2" t="n">
-        <v>106</v>
+        <v>225</v>
       </c>
       <c r="D2" t="n">
-        <v>200</v>
-      </c>
-      <c r="E2" t="n">
-        <v>506</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>shazidmashrafi(Shazid)</t>
+          <t>y_this_kolaveri(SAIF)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D3" t="n">
-        <v>180</v>
-      </c>
-      <c r="E3" t="n">
-        <v>460</v>
+        <v>378</v>
       </c>
     </row>
     <row r="4">
@@ -970,10 +892,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="n">
-        <v>129</v>
-      </c>
-      <c r="E4" t="n">
-        <v>458</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +906,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,20 +922,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -1032,51 +946,42 @@
         <v>164</v>
       </c>
       <c r="C2" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="D2" t="n">
-        <v>164</v>
-      </c>
-      <c r="E2" t="n">
-        <v>423</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Aniksamiul(Anik)</t>
+          <t>rakin_ahsan(Rakin)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C3" t="n">
         <v>180</v>
       </c>
       <c r="D3" t="n">
-        <v>120</v>
-      </c>
-      <c r="E3" t="n">
-        <v>420</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Marufhussain(maruf)</t>
+          <t>farhanshadiq(Farhan)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="C4" t="n">
-        <v>90</v>
+        <v>129</v>
       </c>
       <c r="D4" t="n">
-        <v>150</v>
-      </c>
-      <c r="E4" t="n">
-        <v>390</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +995,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1106,20 +1011,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -1128,58 +1028,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>farhanshadiq(Farhan)</t>
+          <t>Noornabi1770(Noor)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C2" t="n">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D2" t="n">
-        <v>113</v>
-      </c>
-      <c r="E2" t="n">
-        <v>390</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Akash_khan</t>
+          <t>Aniksamiul(Anik)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="C3" t="n">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="D3" t="n">
-        <v>139</v>
-      </c>
-      <c r="E3" t="n">
-        <v>364</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rakin_ahsan(Rakin)</t>
+          <t>Apon_Chowdhury(Apon)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C4" t="n">
-        <v>150</v>
+        <v>113</v>
       </c>
       <c r="D4" t="n">
-        <v>106</v>
-      </c>
-      <c r="E4" t="n">
-        <v>362</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>
@@ -1193,7 +1084,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1209,20 +1100,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -1231,58 +1117,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Apon_Chowdhury(Apon)</t>
+          <t>Marufhussain(maruf)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C2" t="n">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="n">
-        <v>339</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SadmanIshtiak(Sadman)</t>
+          <t>Akash_khan</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C3" t="n">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>95</v>
-      </c>
-      <c r="E3" t="n">
-        <v>319</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Noornabi1770(Noor)</t>
+          <t>SadmanIshtiak(Sadman)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C4" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
-      </c>
-      <c r="E4" t="n">
-        <v>300</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1296,7 +1173,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1312,20 +1189,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>01.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 01.xlsx</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>02.xlsx</t>
+          <t>Rank-ICPC 2025 Team Formation - 02.xlsx</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>03.xlsx</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>FinalPoints</t>
         </is>
@@ -1341,13 +1213,10 @@
         <v>86</v>
       </c>
       <c r="C2" t="n">
-        <v>113</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>86</v>
-      </c>
-      <c r="E2" t="n">
-        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Requirements.txt and install dependencies form main function
</commit_message>
<xml_diff>
--- a/final_teams.xlsx
+++ b/final_teams.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -474,7 +479,10 @@
         <v>300</v>
       </c>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>300</v>
+      </c>
+      <c r="E2" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="3">
@@ -490,39 +498,48 @@
         <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>483</v>
+        <v>225</v>
+      </c>
+      <c r="E3" t="n">
+        <v>708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sf61561(Syed Fahad Mahmud)</t>
+          <t>shazidmashrafi(Shazid)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="C4" t="n">
-        <v>164</v>
+        <v>225</v>
       </c>
       <c r="D4" t="n">
-        <v>464</v>
+        <v>258</v>
+      </c>
+      <c r="E4" t="n">
+        <v>663</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>shazidmashrafi(Shazid)</t>
+          <t>sf61561(Syed Fahad Mahmud)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="C5" t="n">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="D5" t="n">
-        <v>405</v>
+        <v>164</v>
+      </c>
+      <c r="E5" t="n">
+        <v>628</v>
       </c>
     </row>
     <row r="6">
@@ -538,103 +555,124 @@
         <v>120</v>
       </c>
       <c r="D6" t="n">
-        <v>378</v>
+        <v>129</v>
+      </c>
+      <c r="E6" t="n">
+        <v>507</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AL_AMIN_17(Al Amin)</t>
+          <t>Md_Saurob_bhuyan(Noob)</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C7" t="n">
-        <v>200</v>
+        <v>139</v>
       </c>
       <c r="D7" t="n">
-        <v>329</v>
+        <v>180</v>
+      </c>
+      <c r="E7" t="n">
+        <v>483</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Md_Saurob_bhuyan(Noob)</t>
+          <t>rakin_ahsan(Rakin)</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="C8" t="n">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="D8" t="n">
-        <v>303</v>
+        <v>120</v>
+      </c>
+      <c r="E8" t="n">
+        <v>406</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>rakin_ahsan(Rakin)</t>
+          <t>farhanshadiq(Farhan)</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C9" t="n">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="D9" t="n">
-        <v>286</v>
+        <v>139</v>
+      </c>
+      <c r="E9" t="n">
+        <v>381</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>farhanshadiq(Farhan)</t>
+          <t>Aniksamiul(Anik)</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C10" t="n">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D10" t="n">
-        <v>242</v>
+        <v>150</v>
+      </c>
+      <c r="E10" t="n">
+        <v>376</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Noornabi1770(Noor)</t>
+          <t>Akash_khan</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="C11" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>240</v>
+        <v>200</v>
+      </c>
+      <c r="E11" t="n">
+        <v>339</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Aniksamiul(Anik)</t>
+          <t>AL_AMIN_17(Al Amin)</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C12" t="n">
-        <v>106</v>
+        <v>200</v>
       </c>
       <c r="D12" t="n">
-        <v>226</v>
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>329</v>
       </c>
     </row>
     <row r="13">
@@ -650,39 +688,48 @@
         <v>113</v>
       </c>
       <c r="D13" t="n">
-        <v>213</v>
+        <v>113</v>
+      </c>
+      <c r="E13" t="n">
+        <v>326</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Marufhussain(maruf)</t>
+          <t>Noornabi1770(Noor)</t>
         </is>
       </c>
       <c r="B14" t="n">
+        <v>90</v>
+      </c>
+      <c r="C14" t="n">
         <v>150</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" t="n">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Akash_khan</t>
+          <t>Marufhussain(maruf)</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>139</v>
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="16">
@@ -698,6 +745,9 @@
         <v>0</v>
       </c>
       <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
         <v>95</v>
       </c>
     </row>
@@ -714,6 +764,9 @@
         <v>0</v>
       </c>
       <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
         <v>86</v>
       </c>
     </row>
@@ -728,7 +781,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -754,6 +807,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -771,7 +829,10 @@
         <v>300</v>
       </c>
       <c r="D2" t="n">
-        <v>500</v>
+        <v>300</v>
+      </c>
+      <c r="E2" t="n">
+        <v>800</v>
       </c>
     </row>
     <row r="3">
@@ -787,23 +848,29 @@
         <v>258</v>
       </c>
       <c r="D3" t="n">
-        <v>483</v>
+        <v>225</v>
+      </c>
+      <c r="E3" t="n">
+        <v>708</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>sf61561(Syed Fahad Mahmud)</t>
+          <t>shazidmashrafi(Shazid)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>300</v>
+        <v>180</v>
       </c>
       <c r="C4" t="n">
-        <v>164</v>
+        <v>225</v>
       </c>
       <c r="D4" t="n">
-        <v>464</v>
+        <v>258</v>
+      </c>
+      <c r="E4" t="n">
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -817,7 +884,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,6 +910,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -850,17 +922,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>shazidmashrafi(Shazid)</t>
+          <t>sf61561(Syed Fahad Mahmud)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="C2" t="n">
-        <v>225</v>
+        <v>164</v>
       </c>
       <c r="D2" t="n">
-        <v>405</v>
+        <v>164</v>
+      </c>
+      <c r="E2" t="n">
+        <v>628</v>
       </c>
     </row>
     <row r="3">
@@ -876,23 +951,29 @@
         <v>120</v>
       </c>
       <c r="D3" t="n">
-        <v>378</v>
+        <v>129</v>
+      </c>
+      <c r="E3" t="n">
+        <v>507</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AL_AMIN_17(Al Amin)</t>
+          <t>Md_Saurob_bhuyan(Noob)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>129</v>
+        <v>164</v>
       </c>
       <c r="C4" t="n">
-        <v>200</v>
+        <v>139</v>
       </c>
       <c r="D4" t="n">
-        <v>329</v>
+        <v>180</v>
+      </c>
+      <c r="E4" t="n">
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -906,7 +987,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,6 +1013,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -939,49 +1025,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Md_Saurob_bhuyan(Noob)</t>
+          <t>rakin_ahsan(Rakin)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="C2" t="n">
-        <v>139</v>
+        <v>180</v>
       </c>
       <c r="D2" t="n">
-        <v>303</v>
+        <v>120</v>
+      </c>
+      <c r="E2" t="n">
+        <v>406</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rakin_ahsan(Rakin)</t>
+          <t>farhanshadiq(Farhan)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="C3" t="n">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="D3" t="n">
-        <v>286</v>
+        <v>139</v>
+      </c>
+      <c r="E3" t="n">
+        <v>381</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>farhanshadiq(Farhan)</t>
+          <t>Aniksamiul(Anik)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C4" t="n">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D4" t="n">
-        <v>242</v>
+        <v>150</v>
+      </c>
+      <c r="E4" t="n">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -995,7 +1090,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1021,6 +1116,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -1028,33 +1128,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Noornabi1770(Noor)</t>
+          <t>Akash_khan</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90</v>
+        <v>139</v>
       </c>
       <c r="C2" t="n">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>240</v>
+        <v>200</v>
+      </c>
+      <c r="E2" t="n">
+        <v>339</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Aniksamiul(Anik)</t>
+          <t>AL_AMIN_17(Al Amin)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C3" t="n">
-        <v>106</v>
+        <v>200</v>
       </c>
       <c r="D3" t="n">
-        <v>226</v>
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>329</v>
       </c>
     </row>
     <row r="4">
@@ -1070,7 +1176,10 @@
         <v>113</v>
       </c>
       <c r="D4" t="n">
-        <v>213</v>
+        <v>113</v>
+      </c>
+      <c r="E4" t="n">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -1084,7 +1193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,6 +1219,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -1117,33 +1231,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Marufhussain(maruf)</t>
+          <t>Noornabi1770(Noor)</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>90</v>
+      </c>
+      <c r="C2" t="n">
         <v>150</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
-        <v>150</v>
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>240</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Akash_khan</t>
+          <t>Marufhussain(maruf)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>139</v>
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="4">
@@ -1159,6 +1279,9 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>95</v>
       </c>
     </row>
@@ -1173,7 +1296,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1199,6 +1322,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rank-ICPC 2025 Team Formation - 03.xlsx</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FinalPoints</t>
         </is>
       </c>
@@ -1216,6 +1344,9 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
         <v>86</v>
       </c>
     </row>

</xml_diff>